<commit_message>
Se elimino la rama master y se agrego el archivo cronograma al principal
</commit_message>
<xml_diff>
--- a/Proyecto 2 -Estudio de Factibilidad - Grupo 3 - copia.xlsx
+++ b/Proyecto 2 -Estudio de Factibilidad - Grupo 3 - copia.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Proyecto 2\Grupo-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D689C6-07C2-4C16-BCD9-0CBB96D7DBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estudio factibilidad" sheetId="1" r:id="rId1"/>
     <sheet name="Recursos Tecnicos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -225,10 +235,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$₡-140A]* #,##0.00_-;\-[$₡-140A]* #,##0.00_-;_-[$₡-140A]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$₡-140A]* #,##0.00_-;\-[$₡-140A]* #,##0.00_-;_-[$₡-140A]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -937,14 +947,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -952,12 +962,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -966,20 +976,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -998,12 +1008,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1011,7 +1021,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,8 +1037,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1166,45 +1176,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1212,6 +1183,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1229,8 +1209,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1239,6 +1228,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1560,11 +1570,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2015,10 +2025,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:D20"/>
     </sheetView>
   </sheetViews>
@@ -2033,12 +2043,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="111"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="98"/>
       <c r="E1" s="51"/>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -2127,10 +2137,10 @@
       <c r="Z3" s="49"/>
     </row>
     <row r="4" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="99" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="56" t="s">
@@ -2163,8 +2173,8 @@
       <c r="Z4" s="49"/>
     </row>
     <row r="5" spans="1:26" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="119"/>
-      <c r="B5" s="102"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="58" t="s">
         <v>39</v>
       </c>
@@ -2195,8 +2205,8 @@
       <c r="Z5" s="49"/>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="100"/>
+      <c r="A6" s="113"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="60" t="s">
         <v>40</v>
       </c>
@@ -2229,16 +2239,16 @@
       <c r="Z6" s="49"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="105" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="106">
+      <c r="D7" s="118">
         <v>2</v>
       </c>
       <c r="E7" s="51"/>
@@ -2267,12 +2277,12 @@
       <c r="Z7" s="49"/>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="113"/>
-      <c r="B8" s="116"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="107"/>
+      <c r="D8" s="119"/>
       <c r="E8" s="51"/>
       <c r="F8" s="72" t="s">
         <v>60</v>
@@ -2299,12 +2309,12 @@
       <c r="Z8" s="49"/>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="113"/>
-      <c r="B9" s="116"/>
+      <c r="A9" s="103"/>
+      <c r="B9" s="106"/>
       <c r="C9" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="107"/>
+      <c r="D9" s="119"/>
       <c r="E9" s="51"/>
       <c r="F9" s="72" t="s">
         <v>61</v>
@@ -2331,12 +2341,12 @@
       <c r="Z9" s="49"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="113"/>
-      <c r="B10" s="116"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="108"/>
+      <c r="D10" s="120"/>
       <c r="E10" s="51"/>
       <c r="F10" s="72" t="s">
         <v>62</v>
@@ -2363,7 +2373,7 @@
       <c r="Z10" s="49"/>
     </row>
     <row r="11" spans="1:26" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="114"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="63" t="s">
         <v>46</v>
       </c>
@@ -2399,16 +2409,16 @@
       <c r="Z11" s="49"/>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="112" t="s">
+      <c r="A12" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="97" t="s">
+      <c r="B12" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="98">
+      <c r="D12" s="115">
         <v>3</v>
       </c>
       <c r="E12" s="51"/>
@@ -2435,10 +2445,10 @@
       <c r="Z12" s="49"/>
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="113"/>
-      <c r="B13" s="102"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="105"/>
+      <c r="A13" s="103"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="109"/>
       <c r="E13" s="51"/>
       <c r="F13" s="49"/>
       <c r="G13" s="49"/>
@@ -2463,7 +2473,7 @@
       <c r="Z13" s="49"/>
     </row>
     <row r="14" spans="1:26" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="113"/>
+      <c r="A14" s="103"/>
       <c r="B14" s="66" t="s">
         <v>50</v>
       </c>
@@ -2497,7 +2507,7 @@
       <c r="Z14" s="49"/>
     </row>
     <row r="15" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
+      <c r="A15" s="103"/>
       <c r="B15" s="66" t="s">
         <v>52</v>
       </c>
@@ -2531,7 +2541,7 @@
       <c r="Z15" s="49"/>
     </row>
     <row r="16" spans="1:26" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="113"/>
+      <c r="A16" s="103"/>
       <c r="B16" s="58" t="s">
         <v>54</v>
       </c>
@@ -2565,14 +2575,14 @@
       <c r="Z16" s="49"/>
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="113"/>
-      <c r="B17" s="102" t="s">
+      <c r="A17" s="103"/>
+      <c r="B17" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="105">
+      <c r="D17" s="109">
         <v>1</v>
       </c>
       <c r="E17" s="51"/>
@@ -2599,10 +2609,10 @@
       <c r="Z17" s="49"/>
     </row>
     <row r="18" spans="1:26" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="114"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="101"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="110"/>
       <c r="E18" s="51"/>
       <c r="F18" s="49"/>
       <c r="G18" s="49"/>
@@ -2627,12 +2637,12 @@
       <c r="Z18" s="49"/>
     </row>
     <row r="19" spans="1:26" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="96" t="s">
+      <c r="A19" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="97"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="98"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="115"/>
       <c r="E19" s="51"/>
       <c r="F19" s="49"/>
       <c r="G19" s="49"/>
@@ -2657,10 +2667,10 @@
       <c r="Z19" s="49"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="99"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="101"/>
+      <c r="A20" s="116"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="110"/>
       <c r="E20" s="51"/>
       <c r="F20" s="49"/>
       <c r="G20" s="49"/>
@@ -30154,6 +30164,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A19:D20"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D7:D10"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="A7:A11"/>
@@ -30163,11 +30178,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A19:D20"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D7:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>